<commit_message>
+Changes in the process transaction
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shireen.M\Documents\UiPath\Day10_Assignment1\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Documents\UiPath\Shireen_Day_10_1\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{098D5668-41AB-4486-BACF-1810A77CB4E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F0EF503-E10D-4946-8CD2-2388DA1EB883}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="50">
   <si>
     <t>Name</t>
   </si>
@@ -163,6 +163,18 @@
   </si>
   <si>
     <t>InputDetails</t>
+  </si>
+  <si>
+    <t>InputDataFile</t>
+  </si>
+  <si>
+    <t>C:\Users\hp\Documents\UiPath\Shireen_Day_10_1\Data\Input\input_Unicorn_names.xlsx</t>
+  </si>
+  <si>
+    <t>InputDataSheet</t>
+  </si>
+  <si>
+    <t>Sheet1</t>
   </si>
 </sst>
 </file>
@@ -242,9 +254,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -282,7 +294,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -388,7 +400,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -530,7 +542,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -540,16 +552,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" customWidth="1"/>
+    <col min="1" max="1" width="43.54296875" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="81.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -597,7 +609,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="45">
+    <row r="3" spans="1:26" ht="43.5">
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
@@ -609,7 +621,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="30">
+    <row r="5" spans="1:26" ht="29">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1624,16 +1636,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
-    <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="2" max="2" width="60.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="75.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1670,7 +1682,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="30">
+    <row r="2" spans="1:26" ht="29">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1681,7 +1693,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="45">
+    <row r="3" spans="1:26" ht="43.5">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -1795,7 +1807,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="45">
+    <row r="17" spans="1:3" ht="29">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -1806,8 +1818,22 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="18" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A19" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" t="s">
+        <v>49</v>
+      </c>
+    </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2789,12 +2815,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" customWidth="1"/>
-    <col min="3" max="3" width="60.28515625" customWidth="1"/>
-    <col min="4" max="26" width="65.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.81640625" customWidth="1"/>
+    <col min="2" max="2" width="30.1796875" customWidth="1"/>
+    <col min="3" max="3" width="60.26953125" customWidth="1"/>
+    <col min="4" max="26" width="65.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
+Completed the question with annotations
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Documents\UiPath\Shireen_Day_10_1\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shireen.M\Documents\UiPath\Shireen_Day_10_final\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F0EF503-E10D-4946-8CD2-2388DA1EB883}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D23D3331-CECF-4516-B961-8B06056E6527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="69">
   <si>
     <t>Name</t>
   </si>
@@ -98,83 +98,139 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
+    <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction succesful.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction failed with business exception.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction failed with application exception.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Calling Get Transaction Data.</t>
+  </si>
+  <si>
+    <t>OrchestratorAssetFolder</t>
+  </si>
+  <si>
+    <t>OrchestratorQueueFolder</t>
+  </si>
+  <si>
+    <t>Folder name. The value must match a folder defined in Orchestrator and queue specified as OrchestratorQueueName should be created in this folder. For classic folders leave the value field empty.</t>
+  </si>
+  <si>
+    <t>MaxConsecutiveSystemExceptions</t>
+  </si>
+  <si>
+    <t>ExceptionMessage_ConsecutiveErrors</t>
+  </si>
+  <si>
+    <t>RetryNumberGetTransactionItem</t>
+  </si>
+  <si>
+    <t>RetryNumberSetTransactionStatus</t>
+  </si>
+  <si>
+    <t>Error message in case MaxConsecutiveSystemExceptions number is reached.</t>
+  </si>
+  <si>
+    <t>The number of times Get Transaction Item activity is retried in case of an exception. Must be an integer &gt;= 1.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of times Set transaction status activity is retried in case of an exception. Must be an integer &gt;= 1. </t>
+  </si>
+  <si>
+    <t>ShouldMarkJobAsFaulted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of consecutive system exceptions allowed. If MaxConsecutiveSystemExceptions is reached, the job is stopped. To disable this feature, set the value to 0. </t>
+  </si>
+  <si>
+    <t>Must be TRUE or FALSE. If the value is TRUE and an error occurs in Initialization state or the MaxConsecutiveSystemExceptions is reached, the job is marked as Faulted.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
+  </si>
+  <si>
+    <t>Training</t>
+  </si>
+  <si>
+    <t>InputDetails</t>
+  </si>
+  <si>
+    <t>InputDataFile</t>
+  </si>
+  <si>
+    <t>InputDataSheet</t>
+  </si>
+  <si>
+    <t>Sheet1</t>
+  </si>
+  <si>
+    <t>Data\Input\input_Unicorn_names.xlsx</t>
+  </si>
+  <si>
+    <t>BrowserPath</t>
+  </si>
+  <si>
+    <t>http://www.rpasamples.com/unicornname</t>
+  </si>
+  <si>
+    <t>TimeOut</t>
+  </si>
+  <si>
     <t>OrchestratorQueueName</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction succesful.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction failed with business exception.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction failed with application exception.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Calling Get Transaction Data.</t>
-  </si>
-  <si>
-    <t>OrchestratorAssetFolder</t>
-  </si>
-  <si>
-    <t>OrchestratorQueueFolder</t>
-  </si>
-  <si>
-    <t>Folder name. The value must match a folder defined in Orchestrator and queue specified as OrchestratorQueueName should be created in this folder. For classic folders leave the value field empty.</t>
-  </si>
-  <si>
-    <t>MaxConsecutiveSystemExceptions</t>
-  </si>
-  <si>
-    <t>ExceptionMessage_ConsecutiveErrors</t>
-  </si>
-  <si>
-    <t>RetryNumberGetTransactionItem</t>
-  </si>
-  <si>
-    <t>RetryNumberSetTransactionStatus</t>
-  </si>
-  <si>
-    <t>Error message in case MaxConsecutiveSystemExceptions number is reached.</t>
-  </si>
-  <si>
-    <t>The number of times Get Transaction Item activity is retried in case of an exception. Must be an integer &gt;= 1.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of times Set transaction status activity is retried in case of an exception. Must be an integer &gt;= 1. </t>
-  </si>
-  <si>
-    <t>ShouldMarkJobAsFaulted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of consecutive system exceptions allowed. If MaxConsecutiveSystemExceptions is reached, the job is stopped. To disable this feature, set the value to 0. </t>
-  </si>
-  <si>
-    <t>Must be TRUE or FALSE. If the value is TRUE and an error occurs in Initialization state or the MaxConsecutiveSystemExceptions is reached, the job is marked as Faulted.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
-  </si>
-  <si>
-    <t>Training</t>
-  </si>
-  <si>
-    <t>InputDetails</t>
-  </si>
-  <si>
-    <t>InputDataFile</t>
-  </si>
-  <si>
-    <t>C:\Users\hp\Documents\UiPath\Shireen_Day_10_1\Data\Input\input_Unicorn_names.xlsx</t>
-  </si>
-  <si>
-    <t>InputDataSheet</t>
-  </si>
-  <si>
-    <t>Sheet1</t>
+  </si>
+  <si>
+    <t>OutputDataFile</t>
+  </si>
+  <si>
+    <t>Data\Output\Question1.xlsx</t>
+  </si>
+  <si>
+    <t>OutputDataSheet</t>
+  </si>
+  <si>
+    <t>Sheet2</t>
+  </si>
+  <si>
+    <t>Name of the input file</t>
+  </si>
+  <si>
+    <t>Name o f the input sheet</t>
+  </si>
+  <si>
+    <t>Unicorn browser path</t>
+  </si>
+  <si>
+    <t>Delay period for check app state</t>
+  </si>
+  <si>
+    <t>Name of the output file</t>
+  </si>
+  <si>
+    <t>Name of the output sheet</t>
+  </si>
+  <si>
+    <t>SystemException</t>
+  </si>
+  <si>
+    <t>BusinessException</t>
+  </si>
+  <si>
+    <t>Name and month is incorrect</t>
+  </si>
+  <si>
+    <t>If the business exception occurs , provide this message</t>
+  </si>
+  <si>
+    <t>If the system exception occurs , provide this message</t>
+  </si>
+  <si>
+    <t>Page not loading</t>
   </si>
 </sst>
 </file>
@@ -226,7 +282,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -236,6 +292,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -254,9 +311,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -294,7 +351,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -400,7 +457,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -542,7 +599,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -553,15 +610,15 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.54296875" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.453125" customWidth="1"/>
-    <col min="4" max="26" width="8.7265625" customWidth="1"/>
+    <col min="3" max="3" width="81.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -600,28 +657,28 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.5">
+    <row r="3" spans="1:26" ht="45">
       <c r="A3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="29">
+    <row r="5" spans="1:26" ht="30">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1636,16 +1693,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
-    <col min="2" max="2" width="60.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="75.453125" customWidth="1"/>
-    <col min="4" max="26" width="8.7265625" customWidth="1"/>
+    <col min="2" max="2" width="60.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="75.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1682,7 +1739,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="29">
+    <row r="2" spans="1:26" ht="30">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1690,18 +1747,18 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.5">
+    <row r="3" spans="1:26" ht="45">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1725,7 +1782,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -1747,7 +1804,7 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -1758,7 +1815,7 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
@@ -1769,77 +1826,143 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="29">
+    <row r="17" spans="1:3" ht="45">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B17" t="b">
         <v>0</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B18" t="s">
-        <v>47</v>
+        <v>48</v>
+      </c>
+      <c r="C18" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B19" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A20" t="s">
         <v>49</v>
       </c>
+      <c r="B20" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" t="s">
+        <v>59</v>
+      </c>
     </row>
-    <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A21" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21">
+        <v>5</v>
+      </c>
+      <c r="C21" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A22" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A23" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" t="s">
+        <v>56</v>
+      </c>
+      <c r="C23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A24" t="s">
+        <v>63</v>
+      </c>
+      <c r="B24" t="s">
+        <v>68</v>
+      </c>
+      <c r="C24" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A25" t="s">
+        <v>64</v>
+      </c>
+      <c r="B25" t="s">
+        <v>65</v>
+      </c>
+      <c r="C25" t="s">
+        <v>66</v>
+      </c>
+    </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2815,12 +2938,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.81640625" customWidth="1"/>
-    <col min="2" max="2" width="30.1796875" customWidth="1"/>
-    <col min="3" max="3" width="60.26953125" customWidth="1"/>
-    <col min="4" max="26" width="65.453125" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" customWidth="1"/>
+    <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2831,7 +2954,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>

</xml_diff>